<commit_message>
Update excel fixtures to use new hyperlink format
</commit_message>
<xml_diff>
--- a/cmd/SplitFFISSpreadsheet/fixtures/example_spreadsheet_trailing_plus_sign_cfda.xlsx
+++ b/cmd/SplitFFISSpreadsheet/fixtures/example_spreadsheet_trailing_plus_sign_cfda.xlsx
@@ -1,218 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
-  <si>
-    <t>Competitive Grant Update 24-1</t>
-  </si>
-  <si>
-    <t>January 2, 2024</t>
-  </si>
-  <si>
-    <t>CFDA</t>
-  </si>
-  <si>
-    <t>Opportunity Title</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>Estimated Funding</t>
-  </si>
-  <si>
-    <t>Expected Awards</t>
-  </si>
-  <si>
-    <t>Opportunity Number</t>
-  </si>
-  <si>
-    <t>Eligibility*</t>
-  </si>
-  <si>
-    <t>Due Date</t>
-  </si>
-  <si>
-    <t>Match?</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Tri</t>
-  </si>
-  <si>
-    <t>IHE</t>
-  </si>
-  <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Infrastructure Investment and Jobs Act</t>
-  </si>
-  <si>
-    <t>81.086+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 1</t>
-  </si>
-  <si>
-    <t>Office of Energy Efficiency and Renewable Energy</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ABC-0003065</t>
-    </r>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Inflation Reduction Act</t>
-  </si>
-  <si>
-    <t>10.727+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 2</t>
-  </si>
-  <si>
-    <t>Forest Service</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>USABC-00012</t>
-    </r>
-  </si>
-  <si>
-    <t>81.253+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 3</t>
-  </si>
-  <si>
-    <t>National Energy Technology Laboratory</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ABC-0003032</t>
-    </r>
-  </si>
-  <si>
-    <t>Department of Agriculture</t>
-  </si>
-  <si>
-    <t>02.980+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 4</t>
-  </si>
-  <si>
-    <t>Animal and Plant Health Inspection Service</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ABC-23-0058</t>
-    </r>
-  </si>
-  <si>
-    <t>*Eligibility: S=state governments, L=local governments, Tri=tribal governments, IHE=institutions of higher education, NP=non-profits, O=other/see announcement</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.000"/>
-    <numFmt numFmtId="60" formatCode="&quot;$&quot;#,##0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Helvetica Neue"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="22"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="16"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="15"/>
+      <sz val="12"/>
       <u val="single"/>
-      <sz val="12"/>
-      <color indexed="15"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -590,260 +437,307 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="102">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +810,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="ff000000"/>
@@ -939,56 +833,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>640508</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>16784</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 3" descr="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1">
-          <a:extLst/>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1250108" cy="1260750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2018,544 +1862,667 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" defaultGridColor="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3516" style="1" customWidth="1"/>
-    <col min="7" max="12" width="4.67188" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5" style="1" customWidth="1"/>
-    <col min="15" max="16" width="8.85156" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col width="8" customWidth="1" style="1" min="1" max="1"/>
+    <col width="44.5" customWidth="1" style="1" min="2" max="2"/>
+    <col width="26" customWidth="1" style="1" min="3" max="3"/>
+    <col width="16.3516" customWidth="1" style="1" min="4" max="4"/>
+    <col width="15" customWidth="1" style="1" min="5" max="5"/>
+    <col width="22.3516" customWidth="1" style="1" min="6" max="6"/>
+    <col width="4.67188" customWidth="1" style="1" min="7" max="12"/>
+    <col width="14" customWidth="1" style="1" min="13" max="13"/>
+    <col width="7.5" customWidth="1" style="1" min="14" max="14"/>
+    <col width="8.851559999999999" customWidth="1" style="1" min="15" max="16"/>
+    <col width="8.851559999999999" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="29.1" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="4"/>
-      <c r="N1" t="s" s="8">
+    <row r="1" ht="29.1" customHeight="1" s="83">
+      <c r="A1" s="84" t="n"/>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="85" t="n"/>
+      <c r="E1" s="6" t="n"/>
+      <c r="F1" s="4" t="n"/>
+      <c r="G1" s="7" t="n"/>
+      <c r="H1" s="7" t="n"/>
+      <c r="I1" s="7" t="n"/>
+      <c r="J1" s="7" t="n"/>
+      <c r="K1" s="7" t="n"/>
+      <c r="L1" s="7" t="n"/>
+      <c r="M1" s="4" t="n"/>
+      <c r="N1" s="8" t="inlineStr">
+        <is>
+          <t>Competitive Grant Update 24-1</t>
+        </is>
+      </c>
+      <c r="O1" s="9" t="n"/>
+      <c r="P1" s="10" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" s="83">
+      <c r="A2" s="86" t="n"/>
+      <c r="B2" s="12" t="n"/>
+      <c r="C2" s="12" t="n"/>
+      <c r="D2" s="87" t="n"/>
+      <c r="E2" s="14" t="n"/>
+      <c r="F2" s="12" t="n"/>
+      <c r="G2" s="15" t="n"/>
+      <c r="H2" s="15" t="n"/>
+      <c r="I2" s="15" t="n"/>
+      <c r="J2" s="15" t="n"/>
+      <c r="K2" s="15" t="n"/>
+      <c r="L2" s="15" t="n"/>
+      <c r="M2" s="12" t="n"/>
+      <c r="N2" s="16" t="inlineStr">
+        <is>
+          <t>January 2, 2024</t>
+        </is>
+      </c>
+      <c r="O2" s="9" t="n"/>
+      <c r="P2" s="10" t="n"/>
+    </row>
+    <row r="3" ht="15.95" customHeight="1" s="83">
+      <c r="A3" s="86" t="n"/>
+      <c r="B3" s="12" t="n"/>
+      <c r="C3" s="17" t="n"/>
+      <c r="D3" s="87" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="12" t="n"/>
+      <c r="G3" s="15" t="n"/>
+      <c r="H3" s="15" t="n"/>
+      <c r="I3" s="15" t="n"/>
+      <c r="J3" s="15" t="n"/>
+      <c r="K3" s="15" t="n"/>
+      <c r="L3" s="15" t="n"/>
+      <c r="M3" s="12" t="n"/>
+      <c r="N3" s="15" t="n"/>
+      <c r="O3" s="9" t="n"/>
+      <c r="P3" s="10" t="n"/>
+    </row>
+    <row r="4" ht="15.95" customHeight="1" s="83">
+      <c r="A4" s="86" t="n"/>
+      <c r="B4" s="12" t="n"/>
+      <c r="C4" s="12" t="n"/>
+      <c r="D4" s="87" t="n"/>
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="12" t="n"/>
+      <c r="G4" s="15" t="n"/>
+      <c r="H4" s="15" t="n"/>
+      <c r="I4" s="15" t="n"/>
+      <c r="J4" s="15" t="n"/>
+      <c r="K4" s="15" t="n"/>
+      <c r="L4" s="15" t="n"/>
+      <c r="M4" s="12" t="n"/>
+      <c r="N4" s="15" t="n"/>
+      <c r="O4" s="9" t="n"/>
+      <c r="P4" s="10" t="n"/>
+    </row>
+    <row r="5" ht="15.95" customHeight="1" s="83">
+      <c r="A5" s="86" t="n"/>
+      <c r="B5" s="12" t="n"/>
+      <c r="C5" s="12" t="n"/>
+      <c r="D5" s="87" t="n"/>
+      <c r="E5" s="14" t="n"/>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="15" t="n"/>
+      <c r="H5" s="15" t="n"/>
+      <c r="I5" s="15" t="n"/>
+      <c r="J5" s="15" t="n"/>
+      <c r="K5" s="15" t="n"/>
+      <c r="L5" s="15" t="n"/>
+      <c r="M5" s="12" t="n"/>
+      <c r="N5" s="15" t="n"/>
+      <c r="O5" s="9" t="n"/>
+      <c r="P5" s="10" t="n"/>
+    </row>
+    <row r="6" ht="15.95" customHeight="1" s="83">
+      <c r="A6" s="86" t="n"/>
+      <c r="B6" s="12" t="n"/>
+      <c r="C6" s="12" t="n"/>
+      <c r="D6" s="87" t="n"/>
+      <c r="E6" s="14" t="n"/>
+      <c r="F6" s="12" t="n"/>
+      <c r="G6" s="15" t="n"/>
+      <c r="H6" s="15" t="n"/>
+      <c r="I6" s="15" t="n"/>
+      <c r="J6" s="15" t="n"/>
+      <c r="K6" s="15" t="n"/>
+      <c r="L6" s="15" t="n"/>
+      <c r="M6" s="12" t="n"/>
+      <c r="N6" s="15" t="n"/>
+      <c r="O6" s="9" t="n"/>
+      <c r="P6" s="10" t="n"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1" s="83">
+      <c r="A7" s="88" t="inlineStr">
+        <is>
+          <t>CFDA</t>
+        </is>
+      </c>
+      <c r="B7" s="89" t="inlineStr">
+        <is>
+          <t>Opportunity Title</t>
+        </is>
+      </c>
+      <c r="C7" s="90" t="inlineStr">
+        <is>
+          <t>Agency</t>
+        </is>
+      </c>
+      <c r="D7" s="91" t="inlineStr">
+        <is>
+          <t>Estimated Funding</t>
+        </is>
+      </c>
+      <c r="E7" s="92" t="inlineStr">
+        <is>
+          <t>Expected Awards</t>
+        </is>
+      </c>
+      <c r="F7" s="89" t="inlineStr">
+        <is>
+          <t>Opportunity Number</t>
+        </is>
+      </c>
+      <c r="G7" s="23" t="inlineStr">
+        <is>
+          <t>Eligibility*</t>
+        </is>
+      </c>
+      <c r="H7" s="93" t="n"/>
+      <c r="I7" s="93" t="n"/>
+      <c r="J7" s="93" t="n"/>
+      <c r="K7" s="93" t="n"/>
+      <c r="L7" s="93" t="n"/>
+      <c r="M7" s="91" t="inlineStr">
+        <is>
+          <t>Due Date</t>
+        </is>
+      </c>
+      <c r="N7" s="23" t="inlineStr">
+        <is>
+          <t>Match?</t>
+        </is>
+      </c>
+      <c r="O7" s="9" t="n"/>
+      <c r="P7" s="10" t="n"/>
+    </row>
+    <row r="8" ht="15.95" customHeight="1" s="83">
+      <c r="A8" s="94" t="n"/>
+      <c r="B8" s="93" t="n"/>
+      <c r="C8" s="93" t="n"/>
+      <c r="D8" s="93" t="n"/>
+      <c r="E8" s="93" t="n"/>
+      <c r="F8" s="93" t="n"/>
+      <c r="G8" s="31" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H8" s="31" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="I8" s="31" t="inlineStr">
+        <is>
+          <t>Tri</t>
+        </is>
+      </c>
+      <c r="J8" s="31" t="inlineStr">
+        <is>
+          <t>IHE</t>
+        </is>
+      </c>
+      <c r="K8" s="31" t="inlineStr">
+        <is>
+          <t>NP</t>
+        </is>
+      </c>
+      <c r="L8" s="31" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="M8" s="93" t="n"/>
+      <c r="N8" s="93" t="n"/>
+      <c r="O8" s="33" t="n"/>
+      <c r="P8" s="34" t="n"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1" s="83">
+      <c r="A9" s="35" t="inlineStr">
+        <is>
+          <t>Infrastructure Investment and Jobs Act</t>
+        </is>
+      </c>
+      <c r="B9" s="95" t="n"/>
+      <c r="C9" s="95" t="n"/>
+      <c r="D9" s="96" t="n"/>
+      <c r="E9" s="38" t="n"/>
+      <c r="F9" s="39" t="n"/>
+      <c r="G9" s="40" t="n"/>
+      <c r="H9" s="40" t="n"/>
+      <c r="I9" s="40" t="n"/>
+      <c r="J9" s="40" t="n"/>
+      <c r="K9" s="40" t="n"/>
+      <c r="L9" s="40" t="n"/>
+      <c r="M9" s="41" t="n"/>
+      <c r="N9" s="42" t="n"/>
+      <c r="O9" s="43" t="n"/>
+      <c r="P9" s="44" t="n"/>
+    </row>
+    <row r="10" ht="33.95" customHeight="1" s="83">
+      <c r="A10" s="45" t="inlineStr">
+        <is>
+          <t>81.086+</t>
+        </is>
+      </c>
+      <c r="B10" s="46" t="inlineStr">
+        <is>
+          <t>Example Opportunity 1</t>
+        </is>
+      </c>
+      <c r="C10" s="46" t="inlineStr">
+        <is>
+          <t>Office of Energy Efficiency and Renewable Energy</t>
+        </is>
+      </c>
+      <c r="D10" s="97" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="E10" s="46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" s="48" t="inlineStr">
+        <is>
+          <t>ABC-0003065</t>
+        </is>
+      </c>
+      <c r="G10" s="49" t="n"/>
+      <c r="H10" s="49" t="n"/>
+      <c r="I10" s="49" t="n"/>
+      <c r="J10" s="49" t="n"/>
+      <c r="K10" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L10" s="49" t="n"/>
+      <c r="M10" s="51" t="n">
+        <v>45057</v>
+      </c>
+      <c r="N10" s="52" t="n"/>
+      <c r="O10" s="9" t="n"/>
+      <c r="P10" s="10" t="n"/>
+    </row>
+    <row r="11" ht="15.95" customHeight="1" s="83">
+      <c r="A11" s="98" t="n"/>
+      <c r="B11" s="54" t="n"/>
+      <c r="C11" s="54" t="n"/>
+      <c r="D11" s="99" t="n"/>
+      <c r="E11" s="56" t="n"/>
+      <c r="F11" s="57" t="n"/>
+      <c r="G11" s="58" t="n"/>
+      <c r="H11" s="58" t="n"/>
+      <c r="I11" s="58" t="n"/>
+      <c r="J11" s="58" t="n"/>
+      <c r="K11" s="58" t="n"/>
+      <c r="L11" s="58" t="n"/>
+      <c r="M11" s="59" t="n"/>
+      <c r="N11" s="54" t="n"/>
+      <c r="O11" s="9" t="n"/>
+      <c r="P11" s="10" t="n"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1" s="83">
+      <c r="A12" s="60" t="inlineStr">
+        <is>
+          <t>Inflation Reduction Act</t>
+        </is>
+      </c>
+      <c r="B12" s="93" t="n"/>
+      <c r="C12" s="93" t="n"/>
+      <c r="D12" s="100" t="n"/>
+      <c r="E12" s="63" t="n"/>
+      <c r="F12" s="64" t="n"/>
+      <c r="G12" s="65" t="n"/>
+      <c r="H12" s="65" t="n"/>
+      <c r="I12" s="65" t="n"/>
+      <c r="J12" s="65" t="n"/>
+      <c r="K12" s="65" t="n"/>
+      <c r="L12" s="65" t="n"/>
+      <c r="M12" s="66" t="n"/>
+      <c r="N12" s="67" t="n"/>
+      <c r="O12" s="9" t="n"/>
+      <c r="P12" s="10" t="n"/>
+    </row>
+    <row r="13" ht="16.5" customHeight="1" s="83">
+      <c r="A13" s="45" t="inlineStr">
+        <is>
+          <t>10.727+</t>
+        </is>
+      </c>
+      <c r="B13" s="46" t="inlineStr">
+        <is>
+          <t>Example Opportunity 2</t>
+        </is>
+      </c>
+      <c r="C13" s="46" t="inlineStr">
+        <is>
+          <t>Forest Service</t>
+        </is>
+      </c>
+      <c r="D13" s="97" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="E13" s="68" t="n">
+        <v>200</v>
+      </c>
+      <c r="F13" s="48" t="inlineStr">
+        <is>
+          <t>USABC-00012</t>
+        </is>
+      </c>
+      <c r="G13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M13" s="51" t="n">
+        <v>45079</v>
+      </c>
+      <c r="N13" s="52" t="n"/>
+      <c r="O13" s="9" t="n"/>
+      <c r="P13" s="10" t="n"/>
+    </row>
+    <row r="14" ht="33.95" customHeight="1" s="83">
+      <c r="A14" s="69" t="inlineStr">
+        <is>
+          <t>81.253+</t>
+        </is>
+      </c>
+      <c r="B14" s="70" t="inlineStr">
+        <is>
+          <t>Example Opportunity 3</t>
+        </is>
+      </c>
+      <c r="C14" s="70" t="inlineStr">
+        <is>
+          <t>National Energy Technology Laboratory</t>
+        </is>
+      </c>
+      <c r="D14" s="99" t="n">
         <v>0</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10"/>
+      <c r="E14" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="71" t="inlineStr">
+        <is>
+          <t>ABC-0003032</t>
+        </is>
+      </c>
+      <c r="G14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M14" s="73" t="n">
+        <v>45055</v>
+      </c>
+      <c r="N14" s="70" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O14" s="9" t="n"/>
+      <c r="P14" s="10" t="n"/>
     </row>
-    <row r="2" ht="21" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="12"/>
-      <c r="N2" t="s" s="16">
-        <v>1</v>
-      </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="10"/>
+    <row r="15" ht="15.95" customHeight="1" s="83">
+      <c r="A15" s="98" t="n"/>
+      <c r="B15" s="54" t="n"/>
+      <c r="C15" s="54" t="n"/>
+      <c r="D15" s="99" t="n"/>
+      <c r="E15" s="56" t="n"/>
+      <c r="F15" s="57" t="n"/>
+      <c r="G15" s="58" t="n"/>
+      <c r="H15" s="58" t="n"/>
+      <c r="I15" s="58" t="n"/>
+      <c r="J15" s="58" t="n"/>
+      <c r="K15" s="58" t="n"/>
+      <c r="L15" s="58" t="n"/>
+      <c r="M15" s="59" t="n"/>
+      <c r="N15" s="54" t="n"/>
+      <c r="O15" s="9" t="n"/>
+      <c r="P15" s="10" t="n"/>
     </row>
-    <row r="3" ht="15.95" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10"/>
+    <row r="16" ht="15.35" customHeight="1" s="83">
+      <c r="A16" s="60" t="inlineStr">
+        <is>
+          <t>Department of Agriculture</t>
+        </is>
+      </c>
+      <c r="B16" s="93" t="n"/>
+      <c r="C16" s="93" t="n"/>
+      <c r="D16" s="100" t="n"/>
+      <c r="E16" s="63" t="n"/>
+      <c r="F16" s="64" t="n"/>
+      <c r="G16" s="65" t="n"/>
+      <c r="H16" s="65" t="n"/>
+      <c r="I16" s="65" t="n"/>
+      <c r="J16" s="65" t="n"/>
+      <c r="K16" s="65" t="n"/>
+      <c r="L16" s="65" t="n"/>
+      <c r="M16" s="66" t="n"/>
+      <c r="N16" s="67" t="n"/>
+      <c r="O16" s="9" t="n"/>
+      <c r="P16" s="10" t="n"/>
     </row>
-    <row r="4" ht="15.95" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="10"/>
+    <row r="17" ht="32.25" customHeight="1" s="83">
+      <c r="A17" s="74" t="inlineStr">
+        <is>
+          <t>02.980+</t>
+        </is>
+      </c>
+      <c r="B17" s="75" t="inlineStr">
+        <is>
+          <t>Example Opportunity 4</t>
+        </is>
+      </c>
+      <c r="C17" s="75" t="inlineStr">
+        <is>
+          <t>Animal and Plant Health Inspection Service</t>
+        </is>
+      </c>
+      <c r="D17" s="75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" s="75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F17" s="76" t="inlineStr">
+        <is>
+          <t>ABC-23-0058</t>
+        </is>
+      </c>
+      <c r="G17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H17" s="78" t="n"/>
+      <c r="I17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K17" s="78" t="n"/>
+      <c r="L17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M17" s="79" t="n">
+        <v>45089</v>
+      </c>
+      <c r="N17" s="80" t="n"/>
+      <c r="O17" s="9" t="n"/>
+      <c r="P17" s="10" t="n"/>
     </row>
-    <row r="5" ht="15.95" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" ht="15.95" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="18">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s" s="19">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s" s="20">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s" s="21">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s" s="22">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s" s="19">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s" s="23">
-        <v>8</v>
-      </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="N7" t="s" s="25">
-        <v>10</v>
-      </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
-    </row>
-    <row r="8" ht="15.95" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="27"/>
-      <c r="G8" t="s" s="31">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s" s="31">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s" s="31">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s" s="31">
-        <v>15</v>
-      </c>
-      <c r="L8" t="s" s="31">
-        <v>16</v>
-      </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" t="s" s="35">
-        <v>17</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="44"/>
-    </row>
-    <row r="10" ht="33.95" customHeight="1">
-      <c r="A10" t="s" s="45">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s" s="46">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s" s="46">
-        <v>20</v>
-      </c>
-      <c r="D10" s="47">
-        <v>5000000</v>
-      </c>
-      <c r="E10" t="s" s="46">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s" s="48">
-        <v>22</v>
-      </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="L10" s="49"/>
-      <c r="M10" s="51">
-        <v>45057</v>
-      </c>
-      <c r="N10" s="52"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" ht="15.95" customHeight="1">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" t="s" s="60">
-        <v>24</v>
-      </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="10"/>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" t="s" s="45">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s" s="46">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s" s="46">
-        <v>27</v>
-      </c>
-      <c r="D13" s="47">
-        <v>1000000000</v>
-      </c>
-      <c r="E13" s="68">
-        <v>200</v>
-      </c>
-      <c r="F13" t="s" s="48">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="H13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="I13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="K13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="L13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="M13" s="51">
-        <v>45079</v>
-      </c>
-      <c r="N13" s="52"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" ht="33.95" customHeight="1">
-      <c r="A14" t="s" s="69">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s" s="70">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s" s="70">
-        <v>31</v>
-      </c>
-      <c r="D14" s="55">
-        <v>0</v>
-      </c>
-      <c r="E14" s="56">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s" s="71">
-        <v>32</v>
-      </c>
-      <c r="G14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="H14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="I14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="J14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="K14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="M14" s="73">
-        <v>45055</v>
-      </c>
-      <c r="N14" t="s" s="70">
-        <v>23</v>
-      </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" ht="15.95" customHeight="1">
-      <c r="A15" s="53"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="10"/>
-    </row>
-    <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="60">
-        <v>33</v>
-      </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" ht="32.25" customHeight="1">
-      <c r="A17" t="s" s="74">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s" s="75">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s" s="75">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s" s="75">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s" s="75">
-        <v>21</v>
-      </c>
-      <c r="F17" t="s" s="76">
-        <v>37</v>
-      </c>
-      <c r="G17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="H17" s="78"/>
-      <c r="I17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="J17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="K17" s="78"/>
-      <c r="L17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="M17" s="79">
-        <v>45089</v>
-      </c>
-      <c r="N17" s="80"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" ht="15.95" customHeight="1">
-      <c r="A18" t="s" s="81">
-        <v>38</v>
-      </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="10"/>
+    <row r="18" ht="15.95" customHeight="1" s="83">
+      <c r="A18" s="81" t="inlineStr">
+        <is>
+          <t>*Eligibility: S=state governments, L=local governments, Tri=tribal governments, IHE=institutions of higher education, NP=non-profits, O=other/see announcement</t>
+        </is>
+      </c>
+      <c r="B18" s="101" t="n"/>
+      <c r="C18" s="101" t="n"/>
+      <c r="D18" s="101" t="n"/>
+      <c r="E18" s="101" t="n"/>
+      <c r="F18" s="101" t="n"/>
+      <c r="G18" s="101" t="n"/>
+      <c r="H18" s="101" t="n"/>
+      <c r="I18" s="101" t="n"/>
+      <c r="J18" s="101" t="n"/>
+      <c r="K18" s="101" t="n"/>
+      <c r="L18" s="101" t="n"/>
+      <c r="M18" s="101" t="n"/>
+      <c r="N18" s="101" t="n"/>
+      <c r="O18" s="9" t="n"/>
+      <c r="P18" s="10" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A18:N18"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="G7:L7"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="G7:L7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:A3 C1:P1 C2:N2 C3:L5 A4:A6 M5 O5:P5 C6:P6 A7 C7:G7 M7:P7 G8:L8 O8:P8 A9 D9:P9 C10:C11 A11:A12 D11:P12 C14:C15 A15:A16 D15:P16 C17:P17 A18 O18:P18">
-    <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" text="Notice of intent">
+  <conditionalFormatting sqref="A1:A3 A4:A6 A7 A9 A11:A12 A15:A16 A18 C1:P1 C2:N2 C3:L5 C6:P6 C7:G7 C10:C11 C14:C15 C17:P17 D9:P9 D11:P12 D15:P16 G8:L8 M5 M7:P7 O5:P5 O8:P8 O18:P18">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(A1))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10 A13:A14 C13 A17">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" text="Notice of intent">
+  <conditionalFormatting sqref="A10 A13:A14 A17 C13">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(A10))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:P10 D14:P14">
-    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D10))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="2" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D10))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:P13">
-    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D13))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="2" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D13))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" location="" tooltip="" display="ABC-0003065"/>
-    <hyperlink ref="F13" r:id="rId2" location="" tooltip="" display="USABC-00012"/>
-    <hyperlink ref="F14" r:id="rId3" location="" tooltip="" display="ABC-0003032"/>
-    <hyperlink ref="F17" r:id="rId4" location="" tooltip="" display="ABC-23-0058"/>
+    <hyperlink ref="F10" location="" tooltip="" display="ABC-0003065" r:id="rId1"/>
+    <hyperlink ref="F13" location="" tooltip="" display="USABC-00012" r:id="rId2"/>
+    <hyperlink ref="F14" location="" tooltip="" display="ABC-0003032" r:id="rId3"/>
+    <hyperlink ref="F17" location="" tooltip="" display="ABC-23-0058" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="0" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12 &amp;K000000&amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Support new URL format for hyperlinked cells in FFIS spreadsheets (#730)
* Support parsing new hyperlink format

* Update excel fixtures to use new hyperlink format

* Add tests for hyperlink support
</commit_message>
<xml_diff>
--- a/cmd/SplitFFISSpreadsheet/fixtures/example_spreadsheet_trailing_plus_sign_cfda.xlsx
+++ b/cmd/SplitFFISSpreadsheet/fixtures/example_spreadsheet_trailing_plus_sign_cfda.xlsx
@@ -1,218 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
-  <si>
-    <t>Competitive Grant Update 24-1</t>
-  </si>
-  <si>
-    <t>January 2, 2024</t>
-  </si>
-  <si>
-    <t>CFDA</t>
-  </si>
-  <si>
-    <t>Opportunity Title</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>Estimated Funding</t>
-  </si>
-  <si>
-    <t>Expected Awards</t>
-  </si>
-  <si>
-    <t>Opportunity Number</t>
-  </si>
-  <si>
-    <t>Eligibility*</t>
-  </si>
-  <si>
-    <t>Due Date</t>
-  </si>
-  <si>
-    <t>Match?</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Tri</t>
-  </si>
-  <si>
-    <t>IHE</t>
-  </si>
-  <si>
-    <t>NP</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Infrastructure Investment and Jobs Act</t>
-  </si>
-  <si>
-    <t>81.086+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 1</t>
-  </si>
-  <si>
-    <t>Office of Energy Efficiency and Renewable Energy</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ABC-0003065</t>
-    </r>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Inflation Reduction Act</t>
-  </si>
-  <si>
-    <t>10.727+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 2</t>
-  </si>
-  <si>
-    <t>Forest Service</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>USABC-00012</t>
-    </r>
-  </si>
-  <si>
-    <t>81.253+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 3</t>
-  </si>
-  <si>
-    <t>National Energy Technology Laboratory</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ABC-0003032</t>
-    </r>
-  </si>
-  <si>
-    <t>Department of Agriculture</t>
-  </si>
-  <si>
-    <t>02.980+</t>
-  </si>
-  <si>
-    <t>Example Opportunity 4</t>
-  </si>
-  <si>
-    <t>Animal and Plant Health Inspection Service</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="12"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>ABC-23-0058</t>
-    </r>
-  </si>
-  <si>
-    <t>*Eligibility: S=state governments, L=local governments, Tri=tribal governments, IHE=institutions of higher education, NP=non-profits, O=other/see announcement</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.000"/>
-    <numFmt numFmtId="60" formatCode="&quot;$&quot;#,##0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Helvetica Neue"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="22"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="8"/>
       <sz val="16"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <color indexed="8"/>
       <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color indexed="15"/>
+      <sz val="12"/>
       <u val="single"/>
-      <sz val="12"/>
-      <color indexed="15"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -590,260 +437,307 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="102">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="5" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -916,7 +810,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="ff000000"/>
@@ -939,56 +833,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>640508</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>16784</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 3" descr="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1">
-          <a:extLst/>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1250108" cy="1260750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2018,544 +1862,667 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" defaultGridColor="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.83333" defaultRowHeight="15.95" customHeight="1" outlineLevelRow="0"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.3516" style="1" customWidth="1"/>
-    <col min="7" max="12" width="4.67188" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5" style="1" customWidth="1"/>
-    <col min="15" max="16" width="8.85156" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col width="8" customWidth="1" style="1" min="1" max="1"/>
+    <col width="44.5" customWidth="1" style="1" min="2" max="2"/>
+    <col width="26" customWidth="1" style="1" min="3" max="3"/>
+    <col width="16.3516" customWidth="1" style="1" min="4" max="4"/>
+    <col width="15" customWidth="1" style="1" min="5" max="5"/>
+    <col width="22.3516" customWidth="1" style="1" min="6" max="6"/>
+    <col width="4.67188" customWidth="1" style="1" min="7" max="12"/>
+    <col width="14" customWidth="1" style="1" min="13" max="13"/>
+    <col width="7.5" customWidth="1" style="1" min="14" max="14"/>
+    <col width="8.851559999999999" customWidth="1" style="1" min="15" max="16"/>
+    <col width="8.851559999999999" customWidth="1" style="1" min="17" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="29.1" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="4"/>
-      <c r="N1" t="s" s="8">
+    <row r="1" ht="29.1" customHeight="1" s="83">
+      <c r="A1" s="84" t="n"/>
+      <c r="B1" s="3" t="n"/>
+      <c r="C1" s="4" t="n"/>
+      <c r="D1" s="85" t="n"/>
+      <c r="E1" s="6" t="n"/>
+      <c r="F1" s="4" t="n"/>
+      <c r="G1" s="7" t="n"/>
+      <c r="H1" s="7" t="n"/>
+      <c r="I1" s="7" t="n"/>
+      <c r="J1" s="7" t="n"/>
+      <c r="K1" s="7" t="n"/>
+      <c r="L1" s="7" t="n"/>
+      <c r="M1" s="4" t="n"/>
+      <c r="N1" s="8" t="inlineStr">
+        <is>
+          <t>Competitive Grant Update 24-1</t>
+        </is>
+      </c>
+      <c r="O1" s="9" t="n"/>
+      <c r="P1" s="10" t="n"/>
+    </row>
+    <row r="2" ht="21" customHeight="1" s="83">
+      <c r="A2" s="86" t="n"/>
+      <c r="B2" s="12" t="n"/>
+      <c r="C2" s="12" t="n"/>
+      <c r="D2" s="87" t="n"/>
+      <c r="E2" s="14" t="n"/>
+      <c r="F2" s="12" t="n"/>
+      <c r="G2" s="15" t="n"/>
+      <c r="H2" s="15" t="n"/>
+      <c r="I2" s="15" t="n"/>
+      <c r="J2" s="15" t="n"/>
+      <c r="K2" s="15" t="n"/>
+      <c r="L2" s="15" t="n"/>
+      <c r="M2" s="12" t="n"/>
+      <c r="N2" s="16" t="inlineStr">
+        <is>
+          <t>January 2, 2024</t>
+        </is>
+      </c>
+      <c r="O2" s="9" t="n"/>
+      <c r="P2" s="10" t="n"/>
+    </row>
+    <row r="3" ht="15.95" customHeight="1" s="83">
+      <c r="A3" s="86" t="n"/>
+      <c r="B3" s="12" t="n"/>
+      <c r="C3" s="17" t="n"/>
+      <c r="D3" s="87" t="n"/>
+      <c r="E3" s="14" t="n"/>
+      <c r="F3" s="12" t="n"/>
+      <c r="G3" s="15" t="n"/>
+      <c r="H3" s="15" t="n"/>
+      <c r="I3" s="15" t="n"/>
+      <c r="J3" s="15" t="n"/>
+      <c r="K3" s="15" t="n"/>
+      <c r="L3" s="15" t="n"/>
+      <c r="M3" s="12" t="n"/>
+      <c r="N3" s="15" t="n"/>
+      <c r="O3" s="9" t="n"/>
+      <c r="P3" s="10" t="n"/>
+    </row>
+    <row r="4" ht="15.95" customHeight="1" s="83">
+      <c r="A4" s="86" t="n"/>
+      <c r="B4" s="12" t="n"/>
+      <c r="C4" s="12" t="n"/>
+      <c r="D4" s="87" t="n"/>
+      <c r="E4" s="14" t="n"/>
+      <c r="F4" s="12" t="n"/>
+      <c r="G4" s="15" t="n"/>
+      <c r="H4" s="15" t="n"/>
+      <c r="I4" s="15" t="n"/>
+      <c r="J4" s="15" t="n"/>
+      <c r="K4" s="15" t="n"/>
+      <c r="L4" s="15" t="n"/>
+      <c r="M4" s="12" t="n"/>
+      <c r="N4" s="15" t="n"/>
+      <c r="O4" s="9" t="n"/>
+      <c r="P4" s="10" t="n"/>
+    </row>
+    <row r="5" ht="15.95" customHeight="1" s="83">
+      <c r="A5" s="86" t="n"/>
+      <c r="B5" s="12" t="n"/>
+      <c r="C5" s="12" t="n"/>
+      <c r="D5" s="87" t="n"/>
+      <c r="E5" s="14" t="n"/>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="15" t="n"/>
+      <c r="H5" s="15" t="n"/>
+      <c r="I5" s="15" t="n"/>
+      <c r="J5" s="15" t="n"/>
+      <c r="K5" s="15" t="n"/>
+      <c r="L5" s="15" t="n"/>
+      <c r="M5" s="12" t="n"/>
+      <c r="N5" s="15" t="n"/>
+      <c r="O5" s="9" t="n"/>
+      <c r="P5" s="10" t="n"/>
+    </row>
+    <row r="6" ht="15.95" customHeight="1" s="83">
+      <c r="A6" s="86" t="n"/>
+      <c r="B6" s="12" t="n"/>
+      <c r="C6" s="12" t="n"/>
+      <c r="D6" s="87" t="n"/>
+      <c r="E6" s="14" t="n"/>
+      <c r="F6" s="12" t="n"/>
+      <c r="G6" s="15" t="n"/>
+      <c r="H6" s="15" t="n"/>
+      <c r="I6" s="15" t="n"/>
+      <c r="J6" s="15" t="n"/>
+      <c r="K6" s="15" t="n"/>
+      <c r="L6" s="15" t="n"/>
+      <c r="M6" s="12" t="n"/>
+      <c r="N6" s="15" t="n"/>
+      <c r="O6" s="9" t="n"/>
+      <c r="P6" s="10" t="n"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1" s="83">
+      <c r="A7" s="88" t="inlineStr">
+        <is>
+          <t>CFDA</t>
+        </is>
+      </c>
+      <c r="B7" s="89" t="inlineStr">
+        <is>
+          <t>Opportunity Title</t>
+        </is>
+      </c>
+      <c r="C7" s="90" t="inlineStr">
+        <is>
+          <t>Agency</t>
+        </is>
+      </c>
+      <c r="D7" s="91" t="inlineStr">
+        <is>
+          <t>Estimated Funding</t>
+        </is>
+      </c>
+      <c r="E7" s="92" t="inlineStr">
+        <is>
+          <t>Expected Awards</t>
+        </is>
+      </c>
+      <c r="F7" s="89" t="inlineStr">
+        <is>
+          <t>Opportunity Number</t>
+        </is>
+      </c>
+      <c r="G7" s="23" t="inlineStr">
+        <is>
+          <t>Eligibility*</t>
+        </is>
+      </c>
+      <c r="H7" s="93" t="n"/>
+      <c r="I7" s="93" t="n"/>
+      <c r="J7" s="93" t="n"/>
+      <c r="K7" s="93" t="n"/>
+      <c r="L7" s="93" t="n"/>
+      <c r="M7" s="91" t="inlineStr">
+        <is>
+          <t>Due Date</t>
+        </is>
+      </c>
+      <c r="N7" s="23" t="inlineStr">
+        <is>
+          <t>Match?</t>
+        </is>
+      </c>
+      <c r="O7" s="9" t="n"/>
+      <c r="P7" s="10" t="n"/>
+    </row>
+    <row r="8" ht="15.95" customHeight="1" s="83">
+      <c r="A8" s="94" t="n"/>
+      <c r="B8" s="93" t="n"/>
+      <c r="C8" s="93" t="n"/>
+      <c r="D8" s="93" t="n"/>
+      <c r="E8" s="93" t="n"/>
+      <c r="F8" s="93" t="n"/>
+      <c r="G8" s="31" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="H8" s="31" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="I8" s="31" t="inlineStr">
+        <is>
+          <t>Tri</t>
+        </is>
+      </c>
+      <c r="J8" s="31" t="inlineStr">
+        <is>
+          <t>IHE</t>
+        </is>
+      </c>
+      <c r="K8" s="31" t="inlineStr">
+        <is>
+          <t>NP</t>
+        </is>
+      </c>
+      <c r="L8" s="31" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="M8" s="93" t="n"/>
+      <c r="N8" s="93" t="n"/>
+      <c r="O8" s="33" t="n"/>
+      <c r="P8" s="34" t="n"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1" s="83">
+      <c r="A9" s="35" t="inlineStr">
+        <is>
+          <t>Infrastructure Investment and Jobs Act</t>
+        </is>
+      </c>
+      <c r="B9" s="95" t="n"/>
+      <c r="C9" s="95" t="n"/>
+      <c r="D9" s="96" t="n"/>
+      <c r="E9" s="38" t="n"/>
+      <c r="F9" s="39" t="n"/>
+      <c r="G9" s="40" t="n"/>
+      <c r="H9" s="40" t="n"/>
+      <c r="I9" s="40" t="n"/>
+      <c r="J9" s="40" t="n"/>
+      <c r="K9" s="40" t="n"/>
+      <c r="L9" s="40" t="n"/>
+      <c r="M9" s="41" t="n"/>
+      <c r="N9" s="42" t="n"/>
+      <c r="O9" s="43" t="n"/>
+      <c r="P9" s="44" t="n"/>
+    </row>
+    <row r="10" ht="33.95" customHeight="1" s="83">
+      <c r="A10" s="45" t="inlineStr">
+        <is>
+          <t>81.086+</t>
+        </is>
+      </c>
+      <c r="B10" s="46" t="inlineStr">
+        <is>
+          <t>Example Opportunity 1</t>
+        </is>
+      </c>
+      <c r="C10" s="46" t="inlineStr">
+        <is>
+          <t>Office of Energy Efficiency and Renewable Energy</t>
+        </is>
+      </c>
+      <c r="D10" s="97" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="E10" s="46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" s="48" t="inlineStr">
+        <is>
+          <t>ABC-0003065</t>
+        </is>
+      </c>
+      <c r="G10" s="49" t="n"/>
+      <c r="H10" s="49" t="n"/>
+      <c r="I10" s="49" t="n"/>
+      <c r="J10" s="49" t="n"/>
+      <c r="K10" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L10" s="49" t="n"/>
+      <c r="M10" s="51" t="n">
+        <v>45057</v>
+      </c>
+      <c r="N10" s="52" t="n"/>
+      <c r="O10" s="9" t="n"/>
+      <c r="P10" s="10" t="n"/>
+    </row>
+    <row r="11" ht="15.95" customHeight="1" s="83">
+      <c r="A11" s="98" t="n"/>
+      <c r="B11" s="54" t="n"/>
+      <c r="C11" s="54" t="n"/>
+      <c r="D11" s="99" t="n"/>
+      <c r="E11" s="56" t="n"/>
+      <c r="F11" s="57" t="n"/>
+      <c r="G11" s="58" t="n"/>
+      <c r="H11" s="58" t="n"/>
+      <c r="I11" s="58" t="n"/>
+      <c r="J11" s="58" t="n"/>
+      <c r="K11" s="58" t="n"/>
+      <c r="L11" s="58" t="n"/>
+      <c r="M11" s="59" t="n"/>
+      <c r="N11" s="54" t="n"/>
+      <c r="O11" s="9" t="n"/>
+      <c r="P11" s="10" t="n"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1" s="83">
+      <c r="A12" s="60" t="inlineStr">
+        <is>
+          <t>Inflation Reduction Act</t>
+        </is>
+      </c>
+      <c r="B12" s="93" t="n"/>
+      <c r="C12" s="93" t="n"/>
+      <c r="D12" s="100" t="n"/>
+      <c r="E12" s="63" t="n"/>
+      <c r="F12" s="64" t="n"/>
+      <c r="G12" s="65" t="n"/>
+      <c r="H12" s="65" t="n"/>
+      <c r="I12" s="65" t="n"/>
+      <c r="J12" s="65" t="n"/>
+      <c r="K12" s="65" t="n"/>
+      <c r="L12" s="65" t="n"/>
+      <c r="M12" s="66" t="n"/>
+      <c r="N12" s="67" t="n"/>
+      <c r="O12" s="9" t="n"/>
+      <c r="P12" s="10" t="n"/>
+    </row>
+    <row r="13" ht="16.5" customHeight="1" s="83">
+      <c r="A13" s="45" t="inlineStr">
+        <is>
+          <t>10.727+</t>
+        </is>
+      </c>
+      <c r="B13" s="46" t="inlineStr">
+        <is>
+          <t>Example Opportunity 2</t>
+        </is>
+      </c>
+      <c r="C13" s="46" t="inlineStr">
+        <is>
+          <t>Forest Service</t>
+        </is>
+      </c>
+      <c r="D13" s="97" t="n">
+        <v>1000000000</v>
+      </c>
+      <c r="E13" s="68" t="n">
+        <v>200</v>
+      </c>
+      <c r="F13" s="48" t="inlineStr">
+        <is>
+          <t>USABC-00012</t>
+        </is>
+      </c>
+      <c r="G13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L13" s="50" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M13" s="51" t="n">
+        <v>45079</v>
+      </c>
+      <c r="N13" s="52" t="n"/>
+      <c r="O13" s="9" t="n"/>
+      <c r="P13" s="10" t="n"/>
+    </row>
+    <row r="14" ht="33.95" customHeight="1" s="83">
+      <c r="A14" s="69" t="inlineStr">
+        <is>
+          <t>81.253+</t>
+        </is>
+      </c>
+      <c r="B14" s="70" t="inlineStr">
+        <is>
+          <t>Example Opportunity 3</t>
+        </is>
+      </c>
+      <c r="C14" s="70" t="inlineStr">
+        <is>
+          <t>National Energy Technology Laboratory</t>
+        </is>
+      </c>
+      <c r="D14" s="99" t="n">
         <v>0</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="10"/>
+      <c r="E14" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="71" t="inlineStr">
+        <is>
+          <t>ABC-0003032</t>
+        </is>
+      </c>
+      <c r="G14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="L14" s="72" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M14" s="73" t="n">
+        <v>45055</v>
+      </c>
+      <c r="N14" s="70" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O14" s="9" t="n"/>
+      <c r="P14" s="10" t="n"/>
     </row>
-    <row r="2" ht="21" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="12"/>
-      <c r="N2" t="s" s="16">
-        <v>1</v>
-      </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="10"/>
+    <row r="15" ht="15.95" customHeight="1" s="83">
+      <c r="A15" s="98" t="n"/>
+      <c r="B15" s="54" t="n"/>
+      <c r="C15" s="54" t="n"/>
+      <c r="D15" s="99" t="n"/>
+      <c r="E15" s="56" t="n"/>
+      <c r="F15" s="57" t="n"/>
+      <c r="G15" s="58" t="n"/>
+      <c r="H15" s="58" t="n"/>
+      <c r="I15" s="58" t="n"/>
+      <c r="J15" s="58" t="n"/>
+      <c r="K15" s="58" t="n"/>
+      <c r="L15" s="58" t="n"/>
+      <c r="M15" s="59" t="n"/>
+      <c r="N15" s="54" t="n"/>
+      <c r="O15" s="9" t="n"/>
+      <c r="P15" s="10" t="n"/>
     </row>
-    <row r="3" ht="15.95" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10"/>
+    <row r="16" ht="15.35" customHeight="1" s="83">
+      <c r="A16" s="60" t="inlineStr">
+        <is>
+          <t>Department of Agriculture</t>
+        </is>
+      </c>
+      <c r="B16" s="93" t="n"/>
+      <c r="C16" s="93" t="n"/>
+      <c r="D16" s="100" t="n"/>
+      <c r="E16" s="63" t="n"/>
+      <c r="F16" s="64" t="n"/>
+      <c r="G16" s="65" t="n"/>
+      <c r="H16" s="65" t="n"/>
+      <c r="I16" s="65" t="n"/>
+      <c r="J16" s="65" t="n"/>
+      <c r="K16" s="65" t="n"/>
+      <c r="L16" s="65" t="n"/>
+      <c r="M16" s="66" t="n"/>
+      <c r="N16" s="67" t="n"/>
+      <c r="O16" s="9" t="n"/>
+      <c r="P16" s="10" t="n"/>
     </row>
-    <row r="4" ht="15.95" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="10"/>
+    <row r="17" ht="32.25" customHeight="1" s="83">
+      <c r="A17" s="74" t="inlineStr">
+        <is>
+          <t>02.980+</t>
+        </is>
+      </c>
+      <c r="B17" s="75" t="inlineStr">
+        <is>
+          <t>Example Opportunity 4</t>
+        </is>
+      </c>
+      <c r="C17" s="75" t="inlineStr">
+        <is>
+          <t>Animal and Plant Health Inspection Service</t>
+        </is>
+      </c>
+      <c r="D17" s="75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" s="75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F17" s="76" t="inlineStr">
+        <is>
+          <t>ABC-23-0058</t>
+        </is>
+      </c>
+      <c r="G17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H17" s="78" t="n"/>
+      <c r="I17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="J17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="K17" s="78" t="n"/>
+      <c r="L17" s="77" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="M17" s="79" t="n">
+        <v>45089</v>
+      </c>
+      <c r="N17" s="80" t="n"/>
+      <c r="O17" s="9" t="n"/>
+      <c r="P17" s="10" t="n"/>
     </row>
-    <row r="5" ht="15.95" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" ht="15.95" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="18">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s" s="19">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s" s="20">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s" s="21">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s" s="22">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s" s="19">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s" s="23">
-        <v>8</v>
-      </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="N7" t="s" s="25">
-        <v>10</v>
-      </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="10"/>
-    </row>
-    <row r="8" ht="15.95" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="27"/>
-      <c r="G8" t="s" s="31">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s" s="31">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s" s="31">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s" s="31">
-        <v>15</v>
-      </c>
-      <c r="L8" t="s" s="31">
-        <v>16</v>
-      </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" t="s" s="35">
-        <v>17</v>
-      </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="44"/>
-    </row>
-    <row r="10" ht="33.95" customHeight="1">
-      <c r="A10" t="s" s="45">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s" s="46">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s" s="46">
-        <v>20</v>
-      </c>
-      <c r="D10" s="47">
-        <v>5000000</v>
-      </c>
-      <c r="E10" t="s" s="46">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s" s="48">
-        <v>22</v>
-      </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="L10" s="49"/>
-      <c r="M10" s="51">
-        <v>45057</v>
-      </c>
-      <c r="N10" s="52"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="10"/>
-    </row>
-    <row r="11" ht="15.95" customHeight="1">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="10"/>
-    </row>
-    <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" t="s" s="60">
-        <v>24</v>
-      </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="65"/>
-      <c r="L12" s="65"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="10"/>
-    </row>
-    <row r="13" ht="16.5" customHeight="1">
-      <c r="A13" t="s" s="45">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s" s="46">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s" s="46">
-        <v>27</v>
-      </c>
-      <c r="D13" s="47">
-        <v>1000000000</v>
-      </c>
-      <c r="E13" s="68">
-        <v>200</v>
-      </c>
-      <c r="F13" t="s" s="48">
-        <v>28</v>
-      </c>
-      <c r="G13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="H13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="I13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="K13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="L13" t="s" s="50">
-        <v>23</v>
-      </c>
-      <c r="M13" s="51">
-        <v>45079</v>
-      </c>
-      <c r="N13" s="52"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" ht="33.95" customHeight="1">
-      <c r="A14" t="s" s="69">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s" s="70">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s" s="70">
-        <v>31</v>
-      </c>
-      <c r="D14" s="55">
-        <v>0</v>
-      </c>
-      <c r="E14" s="56">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s" s="71">
-        <v>32</v>
-      </c>
-      <c r="G14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="H14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="I14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="J14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="K14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s" s="72">
-        <v>23</v>
-      </c>
-      <c r="M14" s="73">
-        <v>45055</v>
-      </c>
-      <c r="N14" t="s" s="70">
-        <v>23</v>
-      </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" ht="15.95" customHeight="1">
-      <c r="A15" s="53"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="10"/>
-    </row>
-    <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="60">
-        <v>33</v>
-      </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" ht="32.25" customHeight="1">
-      <c r="A17" t="s" s="74">
-        <v>34</v>
-      </c>
-      <c r="B17" t="s" s="75">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s" s="75">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s" s="75">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s" s="75">
-        <v>21</v>
-      </c>
-      <c r="F17" t="s" s="76">
-        <v>37</v>
-      </c>
-      <c r="G17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="H17" s="78"/>
-      <c r="I17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="J17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="K17" s="78"/>
-      <c r="L17" t="s" s="77">
-        <v>23</v>
-      </c>
-      <c r="M17" s="79">
-        <v>45089</v>
-      </c>
-      <c r="N17" s="80"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" ht="15.95" customHeight="1">
-      <c r="A18" t="s" s="81">
-        <v>38</v>
-      </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="82"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="10"/>
+    <row r="18" ht="15.95" customHeight="1" s="83">
+      <c r="A18" s="81" t="inlineStr">
+        <is>
+          <t>*Eligibility: S=state governments, L=local governments, Tri=tribal governments, IHE=institutions of higher education, NP=non-profits, O=other/see announcement</t>
+        </is>
+      </c>
+      <c r="B18" s="101" t="n"/>
+      <c r="C18" s="101" t="n"/>
+      <c r="D18" s="101" t="n"/>
+      <c r="E18" s="101" t="n"/>
+      <c r="F18" s="101" t="n"/>
+      <c r="G18" s="101" t="n"/>
+      <c r="H18" s="101" t="n"/>
+      <c r="I18" s="101" t="n"/>
+      <c r="J18" s="101" t="n"/>
+      <c r="K18" s="101" t="n"/>
+      <c r="L18" s="101" t="n"/>
+      <c r="M18" s="101" t="n"/>
+      <c r="N18" s="101" t="n"/>
+      <c r="O18" s="9" t="n"/>
+      <c r="P18" s="10" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A18:N18"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="G7:L7"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="G7:L7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:A3 C1:P1 C2:N2 C3:L5 A4:A6 M5 O5:P5 C6:P6 A7 C7:G7 M7:P7 G8:L8 O8:P8 A9 D9:P9 C10:C11 A11:A12 D11:P12 C14:C15 A15:A16 D15:P16 C17:P17 A18 O18:P18">
-    <cfRule type="containsText" dxfId="0" priority="1" stopIfTrue="1" text="Notice of intent">
+  <conditionalFormatting sqref="A1:A3 A4:A6 A7 A9 A11:A12 A15:A16 A18 C1:P1 C2:N2 C3:L5 C6:P6 C7:G7 C10:C11 C14:C15 C17:P17 D9:P9 D11:P12 D15:P16 G8:L8 M5 M7:P7 O5:P5 O8:P8 O18:P18">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(A1))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10 A13:A14 C13 A17">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" text="Notice of intent">
+  <conditionalFormatting sqref="A10 A13:A14 A17 C13">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(A10))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:P10 D14:P14">
-    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D10))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="2" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D10))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:P13">
-    <cfRule type="containsText" dxfId="4" priority="1" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="1" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D13))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" text="Notice of intent">
+    <cfRule type="containsText" priority="2" dxfId="0" stopIfTrue="1" text="Notice of intent">
       <formula>NOT(ISERROR(FIND(UPPER("Notice of intent"),UPPER(D13))))</formula>
       <formula>"Notice of intent"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" location="" tooltip="" display="ABC-0003065"/>
-    <hyperlink ref="F13" r:id="rId2" location="" tooltip="" display="USABC-00012"/>
-    <hyperlink ref="F14" r:id="rId3" location="" tooltip="" display="ABC-0003032"/>
-    <hyperlink ref="F17" r:id="rId4" location="" tooltip="" display="ABC-23-0058"/>
+    <hyperlink ref="F10" location="" tooltip="" display="ABC-0003065" r:id="rId1"/>
+    <hyperlink ref="F13" location="" tooltip="" display="USABC-00012" r:id="rId2"/>
+    <hyperlink ref="F14" location="" tooltip="" display="ABC-0003032" r:id="rId3"/>
+    <hyperlink ref="F17" location="" tooltip="" display="ABC-23-0058" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="0" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12 &amp;K000000&amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>